<commit_message>
Added feature_selection to randomForest
Added:
updated classifier, readme with summary and report excel file
</commit_message>
<xml_diff>
--- a/classifiers/github_labels/randomforest/report.xlsx
+++ b/classifiers/github_labels/randomforest/report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17668"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="16">
   <si>
     <t>training size</t>
   </si>
@@ -46,13 +46,34 @@
   </si>
   <si>
     <t>90 by 5</t>
+  </si>
+  <si>
+    <t>test data size</t>
+  </si>
+  <si>
+    <t>training data size</t>
+  </si>
+  <si>
+    <t>memory usage</t>
+  </si>
+  <si>
+    <t>Processor usage</t>
+  </si>
+  <si>
+    <t>90 by 100</t>
+  </si>
+  <si>
+    <t>features_percentile</t>
+  </si>
+  <si>
+    <t>90 by 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,8 +95,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,8 +120,43 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -116,18 +179,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="6">
+    <cellStyle name="40% - Accent2" xfId="3" builtinId="35"/>
+    <cellStyle name="40% - Accent6" xfId="5" builtinId="51"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="2" builtinId="10"/>
@@ -143,6 +231,160 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="419100" y="1285875"/>
+          <a:ext cx="7667625" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>going</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> for case 1, 90 by 10, n_estimators = 15, criterion = entropy, last known accuracy = 78.27</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>771525</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="542925" y="5962650"/>
+          <a:ext cx="8896350" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Got a marginal improvement in accuracy but a decent improvement in training time.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -408,82 +650,675 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="I30" sqref="A1:I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="1" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
+      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
         <v>22</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.5</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>78.27</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2">
         <v>56</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>36.6</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>79.739999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1077</v>
+      </c>
+      <c r="F4">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="G4" s="6">
+        <v>85.74</v>
+      </c>
+      <c r="H4">
+        <v>102052</v>
+      </c>
+      <c r="I4">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>0.42154999999999998</v>
+      </c>
+      <c r="F5">
+        <v>0.37</v>
+      </c>
+      <c r="G5">
+        <v>74.25</v>
+      </c>
+      <c r="H5">
+        <v>1020</v>
+      </c>
+      <c r="I5">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>23</v>
+      </c>
+      <c r="F6">
+        <v>0.53</v>
+      </c>
+      <c r="G6">
+        <v>78.459999999999994</v>
+      </c>
+      <c r="H6">
+        <v>10205</v>
+      </c>
+      <c r="I6">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="F11">
+        <v>5.4454000000000002E-2</v>
+      </c>
+      <c r="G11">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="H11">
+        <v>10205</v>
+      </c>
+      <c r="I11">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>1.2</v>
+      </c>
+      <c r="F12">
+        <v>0.161</v>
+      </c>
+      <c r="G12">
+        <v>76.95</v>
+      </c>
+      <c r="H12">
+        <v>10205</v>
+      </c>
+      <c r="I12">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>1.99</v>
+      </c>
+      <c r="F13">
+        <v>0.2</v>
+      </c>
+      <c r="G13">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="H13">
+        <v>10205</v>
+      </c>
+      <c r="I13">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="7">
+        <v>3.56</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="G14" s="7">
+        <v>78.253</v>
+      </c>
+      <c r="H14">
+        <v>10205</v>
+      </c>
+      <c r="I14">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="8">
+        <v>75</v>
+      </c>
+      <c r="C15" s="8">
+        <v>15</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="8">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.36</v>
+      </c>
+      <c r="G15" s="8">
+        <v>78.430000000000007</v>
+      </c>
+      <c r="H15">
+        <v>10205</v>
+      </c>
+      <c r="I15">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>85</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="7">
+        <v>4.3</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0.38</v>
+      </c>
+      <c r="G16" s="7">
+        <v>78.13</v>
+      </c>
+      <c r="H16">
+        <v>10205</v>
+      </c>
+      <c r="I16">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>80</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="7">
+        <v>4.28</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0.36</v>
+      </c>
+      <c r="G17" s="7">
+        <v>78.28</v>
+      </c>
+      <c r="H17">
+        <v>10205</v>
+      </c>
+      <c r="I17">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="G21" s="7">
+        <v>79.7</v>
+      </c>
+      <c r="H21">
+        <v>102052</v>
+      </c>
+      <c r="I21">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="8">
+        <v>33.4</v>
+      </c>
+      <c r="F22" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="G22" s="10">
+        <v>83.76</v>
+      </c>
+      <c r="H22">
+        <v>102052</v>
+      </c>
+      <c r="I22">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>15</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23">
+        <v>56</v>
+      </c>
+      <c r="F23">
+        <v>0.4</v>
+      </c>
+      <c r="G23">
+        <v>84.01</v>
+      </c>
+      <c r="H23">
+        <v>102052</v>
+      </c>
+      <c r="I23">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24">
+        <v>50</v>
+      </c>
+      <c r="C24">
+        <v>15</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24">
+        <v>97</v>
+      </c>
+      <c r="F24">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G24">
+        <v>85.32</v>
+      </c>
+      <c r="H24">
+        <v>102052</v>
+      </c>
+      <c r="I24">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25">
+        <v>75</v>
+      </c>
+      <c r="C25">
+        <v>15</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25">
+        <v>123</v>
+      </c>
+      <c r="F25">
+        <v>0.76</v>
+      </c>
+      <c r="G25">
+        <v>85.41</v>
+      </c>
+      <c r="H25">
+        <v>102052</v>
+      </c>
+      <c r="I25">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26">
+        <v>80</v>
+      </c>
+      <c r="C26">
+        <v>15</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26">
+        <v>125.4</v>
+      </c>
+      <c r="F26">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="G26">
+        <v>85.55</v>
+      </c>
+      <c r="H26">
+        <v>102052</v>
+      </c>
+      <c r="I26">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27">
+        <v>85</v>
+      </c>
+      <c r="C27">
+        <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27">
+        <v>126.54</v>
+      </c>
+      <c r="F27">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="G27">
+        <v>85.52</v>
+      </c>
+      <c r="H27">
+        <v>102052</v>
+      </c>
+      <c r="I27">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="8">
+        <v>90</v>
+      </c>
+      <c r="C28" s="8">
+        <v>15</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="8">
+        <v>127.8</v>
+      </c>
+      <c r="F28" s="8">
+        <v>0.84</v>
+      </c>
+      <c r="G28" s="8">
+        <v>85.71</v>
+      </c>
+      <c r="H28">
+        <v>102052</v>
+      </c>
+      <c r="I28">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="8">
+        <v>95</v>
+      </c>
+      <c r="C29" s="8">
+        <v>15</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="8">
+        <v>129</v>
+      </c>
+      <c r="F29" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="G29" s="8">
+        <v>85.8</v>
+      </c>
+      <c r="H29">
+        <v>102052</v>
+      </c>
+      <c r="I29">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30">
+        <v>100</v>
+      </c>
+      <c r="C30">
+        <v>15</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30">
+        <v>130</v>
+      </c>
+      <c r="F30">
+        <v>0.86</v>
+      </c>
+      <c r="G30">
+        <v>0.85219999999999996</v>
+      </c>
+      <c r="H30">
+        <v>102052</v>
+      </c>
+      <c r="I30">
+        <v>11340</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added updated classifier codes and reports
primarily for syncing work on powerful device. Unable to perform
GridSearchCV on self machine.
</commit_message>
<xml_diff>
--- a/classifiers/github_labels/randomforest/report.xlsx
+++ b/classifiers/github_labels/randomforest/report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="25">
   <si>
     <t>training size</t>
   </si>
@@ -54,12 +54,6 @@
     <t>training data size</t>
   </si>
   <si>
-    <t>memory usage</t>
-  </si>
-  <si>
-    <t>Processor usage</t>
-  </si>
-  <si>
     <t>90 by 100</t>
   </si>
   <si>
@@ -67,6 +61,39 @@
   </si>
   <si>
     <t>90 by 1</t>
+  </si>
+  <si>
+    <t>precision</t>
+  </si>
+  <si>
+    <t>recall</t>
+  </si>
+  <si>
+    <t>fbeta score</t>
+  </si>
+  <si>
+    <t>90  by 1</t>
+  </si>
+  <si>
+    <t>[ 0.87, 0.82]</t>
+  </si>
+  <si>
+    <t>[ 0.92,0.74]</t>
+  </si>
+  <si>
+    <t>[ 0.89,0.78]</t>
+  </si>
+  <si>
+    <t>[0.87, 0.82]</t>
+  </si>
+  <si>
+    <t>[0.92, 0.73]</t>
+  </si>
+  <si>
+    <t>[0.89, 0.77]</t>
+  </si>
+  <si>
+    <t>not done</t>
   </si>
 </sst>
 </file>
@@ -250,7 +277,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -319,25 +352,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>771525</xdr:colOff>
+      <xdr:colOff>838200</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="542925" y="5962650"/>
-          <a:ext cx="8896350" cy="352425"/>
+          <a:off x="609600" y="5829300"/>
+          <a:ext cx="8896350" cy="561975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -379,6 +418,126 @@
             </a:rPr>
             <a:t>Got a marginal improvement in accuracy but a decent improvement in training time.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Added precision, recall</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> and fbeta score as metrics</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62EE0A79-C080-412C-A687-943363E160E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="590550" y="7372350"/>
+          <a:ext cx="8896350" cy="647700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Performed GridSearchCV</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> to get best parameters for 90 by 10 on 95%ile data. Result was:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>n_estimators = "", criterion="" and min_samples_split = ""</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -650,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="A1:I30"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,16 +824,17 @@
     <col min="6" max="6" width="16.42578125" customWidth="1"/>
     <col min="8" max="8" width="17.28515625" customWidth="1"/>
     <col min="9" max="9" width="18.42578125" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -698,13 +858,16 @@
         <v>9</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -724,7 +887,7 @@
         <v>78.27</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -745,9 +908,9 @@
         <v>79.739999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -772,9 +935,9 @@
         <v>11340</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>15</v>
@@ -798,9 +961,9 @@
         <v>11340</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>15</v>
@@ -824,9 +987,9 @@
         <v>11340</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -853,9 +1016,9 @@
         <v>11340</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -882,9 +1045,9 @@
         <v>11340</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>20</v>
@@ -911,9 +1074,9 @@
         <v>11340</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14">
         <v>50</v>
@@ -940,9 +1103,9 @@
         <v>11340</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" s="8">
         <v>75</v>
@@ -969,9 +1132,9 @@
         <v>11340</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16">
         <v>85</v>
@@ -1000,7 +1163,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B17">
         <v>80</v>
@@ -1029,7 +1192,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1058,7 +1221,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B22">
         <v>10</v>
@@ -1087,7 +1250,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B23">
         <v>20</v>
@@ -1116,7 +1279,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B24">
         <v>50</v>
@@ -1145,7 +1308,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B25">
         <v>75</v>
@@ -1174,7 +1337,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B26">
         <v>80</v>
@@ -1203,7 +1366,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B27">
         <v>85</v>
@@ -1232,7 +1395,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B28" s="8">
         <v>90</v>
@@ -1261,7 +1424,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B29" s="8">
         <v>95</v>
@@ -1290,7 +1453,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B30">
         <v>100</v>
@@ -1315,6 +1478,149 @@
       </c>
       <c r="I30">
         <v>11340</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35">
+        <v>100</v>
+      </c>
+      <c r="C35">
+        <v>15</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35">
+        <v>5.2</v>
+      </c>
+      <c r="F35">
+        <v>0.47</v>
+      </c>
+      <c r="G35">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="H35">
+        <v>10205</v>
+      </c>
+      <c r="I35">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36">
+        <v>100</v>
+      </c>
+      <c r="C36">
+        <v>15</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36">
+        <v>155.15</v>
+      </c>
+      <c r="F36">
+        <v>1.02</v>
+      </c>
+      <c r="G36">
+        <v>85.61</v>
+      </c>
+      <c r="H36">
+        <v>102052</v>
+      </c>
+      <c r="I36">
+        <v>11340</v>
+      </c>
+      <c r="J36" t="s">
+        <v>18</v>
+      </c>
+      <c r="K36" t="s">
+        <v>19</v>
+      </c>
+      <c r="L36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37">
+        <v>95</v>
+      </c>
+      <c r="C37">
+        <v>15</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37">
+        <v>156.91</v>
+      </c>
+      <c r="F37">
+        <v>1.002</v>
+      </c>
+      <c r="G37">
+        <v>85.48</v>
+      </c>
+      <c r="H37">
+        <v>102052</v>
+      </c>
+      <c r="I37">
+        <v>11340</v>
+      </c>
+      <c r="J37" t="s">
+        <v>21</v>
+      </c>
+      <c r="K37" t="s">
+        <v>22</v>
+      </c>
+      <c r="L37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38">
+        <v>15</v>
+      </c>
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38">
+        <v>887.79</v>
+      </c>
+      <c r="F38">
+        <v>0.7</v>
+      </c>
+      <c r="G38">
+        <v>85.34</v>
+      </c>
+      <c r="H38">
+        <v>102052</v>
+      </c>
+      <c r="I38">
+        <v>11340</v>
+      </c>
+      <c r="J38" t="s">
+        <v>21</v>
+      </c>
+      <c r="K38" t="s">
+        <v>22</v>
+      </c>
+      <c r="L38" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated randomforest classifier and report
</commit_message>
<xml_diff>
--- a/classifiers/github_labels/randomforest/report.xlsx
+++ b/classifiers/github_labels/randomforest/report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2250" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="2700" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="26">
   <si>
     <t>training size</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>not done</t>
+  </si>
+  <si>
+    <t>gini</t>
   </si>
 </sst>
 </file>
@@ -130,7 +133,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,6 +185,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -226,7 +235,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
@@ -238,6 +247,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent2" xfId="3" builtinId="35"/>
@@ -456,8 +466,8 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -473,7 +483,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="590550" y="7372350"/>
-          <a:ext cx="8896350" cy="647700"/>
+          <a:ext cx="8896350" cy="1047750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -521,7 +531,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> to get best parameters for 90 by 10 on 95%ile data. Result was:</a:t>
+            <a:t> to get best parameters for 90 by 10 on 95%ile data.  Couldn't perform due to time issues.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -531,7 +541,27 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>n_estimators = "", criterion="" and min_samples_split = ""</a:t>
+            <a:t>Performed on 90 by 100 with 95%ile.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Result was different each time. Based on best case these params were chosen</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>n_estimators = "50", criterion="gini" and min_samples_split = "10" and &lt;50, entropy, 10&gt;</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1400">
             <a:solidFill>
@@ -809,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1623,6 +1653,134 @@
         <v>23</v>
       </c>
     </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46">
+        <v>95</v>
+      </c>
+      <c r="C46">
+        <v>50</v>
+      </c>
+      <c r="D46" t="s">
+        <v>25</v>
+      </c>
+      <c r="E46">
+        <v>10.8</v>
+      </c>
+      <c r="F46">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G46">
+        <v>79.94</v>
+      </c>
+      <c r="H46">
+        <v>10205</v>
+      </c>
+      <c r="I46">
+        <v>11340</v>
+      </c>
+      <c r="J46">
+        <v>0.8</v>
+      </c>
+      <c r="K46">
+        <v>0.8</v>
+      </c>
+      <c r="L46">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47">
+        <v>95</v>
+      </c>
+      <c r="C47">
+        <v>50</v>
+      </c>
+      <c r="D47" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47">
+        <v>10.6</v>
+      </c>
+      <c r="F47">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="G47">
+        <v>79.900000000000006</v>
+      </c>
+      <c r="H47">
+        <v>10205</v>
+      </c>
+      <c r="I47">
+        <v>11340</v>
+      </c>
+      <c r="J47">
+        <v>0.79</v>
+      </c>
+      <c r="K47">
+        <v>0.8</v>
+      </c>
+      <c r="L47">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" s="11">
+        <v>95</v>
+      </c>
+      <c r="C48" s="11">
+        <v>50</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11">
+        <v>102052</v>
+      </c>
+      <c r="I48" s="11">
+        <v>11340</v>
+      </c>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="11">
+        <v>95</v>
+      </c>
+      <c r="C49" s="11">
+        <v>50</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11">
+        <v>102052</v>
+      </c>
+      <c r="I49" s="11">
+        <v>11340</v>
+      </c>
+      <c r="J49" s="11"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="11"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>